<commit_message>
feat: updated rss urls
</commit_message>
<xml_diff>
--- a/rss_urls.xlsx
+++ b/rss_urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projetos\falcon_sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA1B76D-6BE5-4FDE-B998-C3E8EE24FBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F0E53A-11D3-425B-961A-61E9B1266A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4335" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,16 +45,16 @@
     <t>https://www.upwork.com/nx/search/jobs/?client_hires=1-9,10-&amp;nbs=1&amp;payment_verified=1&amp;q=video%20editing&amp;sort=recency</t>
   </si>
   <si>
-    <t>https://www.upwork.com/ab/feed/jobs/rss?client_hires=1-9%2C10-&amp;paging=NaN-undefined&amp;payment_verified=1&amp;q=video%20editing&amp;sort=recency&amp;api_params=1&amp;securityToken=8e30fe0a1b948a9d75b6cad06e68ece000fe1f47a205dde324e8a52a62079811690f4f92859d2401105b2e2265d7a286ab5034302b2790beb21d38bf627d00ce&amp;userUid=1795160827512143872&amp;orgUid=1795160827512143873</t>
-  </si>
-  <si>
-    <t>https://www.upwork.com/nx/search/jobs/?client_hires=1-9,10-&amp;nbs=1&amp;payment_verified=1&amp;q=video%20editor&amp;sort=recency</t>
-  </si>
-  <si>
-    <t>payment verified, 1 to 9 and 10+ hires, worldwide "video editor"</t>
-  </si>
-  <si>
-    <t>https://www.upwork.com/ab/feed/jobs/rss?client_hires=1-9%2C10-&amp;paging=NaN-undefined&amp;payment_verified=1&amp;q=video%20editor&amp;sort=recency&amp;api_params=1&amp;securityToken=8e30fe0a1b948a9d75b6cad06e68ece000fe1f47a205dde324e8a52a62079811690f4f92859d2401105b2e2265d7a286ab5034302b2790beb21d38bf627d00ce&amp;userUid=1795160827512143872&amp;orgUid=1795160827512143873</t>
+    <t>https://www.upwork.com/nx/search/jobs/?client_hires=1-9,10-&amp;nbs=1&amp;payment_verified=1&amp;q=video%20editing&amp;sort=recency&amp;user_location_match=1</t>
+  </si>
+  <si>
+    <t>payment verified, 1 to 9 and 10+ hires, us-only "video editor"</t>
+  </si>
+  <si>
+    <t>https://www.upwork.com/ab/feed/jobs/rss?client_hires=1-9%2C10-&amp;paging=NaN-undefined&amp;payment_verified=1&amp;q=video%20editing&amp;sort=recency&amp;user_location_match=1&amp;api_params=1&amp;securityToken=418adc6b3d5cfe830ce53f53b359cf3ed0874223d1a0521e8482731da9873c591396925763d482d9d7f4595e2a28196fcf5f1af259c8298d64066d1b522d2fdf&amp;userUid=1795161265690873856&amp;orgUid=1795161265690873857</t>
+  </si>
+  <si>
+    <t>https://www.upwork.com/ab/feed/jobs/rss?client_hires=1-9%2C10-&amp;paging=NaN-undefined&amp;payment_verified=1&amp;q=video%20editing&amp;sort=recency&amp;api_params=1&amp;securityToken=418adc6b3d5cfe830ce53f53b359cf3ed0874223d1a0521e8482731da9873c591396925763d482d9d7f4595e2a28196fcf5f1af259c8298d64066d1b522d2fdf&amp;userUid=1795161265690873856&amp;orgUid=1795161265690873857</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -428,19 +428,18 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{B3063A90-2F0B-487E-8B47-83523D275CF7}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{76EC95C2-8FFD-47A5-A545-EE13F07CBB81}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B8706DE6-EED3-4931-83F4-48B127D66FE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>